<commit_message>
Commiting changes made to ripples for Louvain-imm
</commit_message>
<xml_diff>
--- a/NewExpts/Time/Results.xlsx
+++ b/NewExpts/Time/Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reetb\Desktop\Louvain-InfMax\NewExpts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reetb\Desktop\Louvain-InfMax\NewExpts\Time\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E5312D2-C55F-493D-A7DD-D979239E937E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C038E1-42B8-48DC-9E95-158EA68EF011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57600" yWindow="3750" windowWidth="9600" windowHeight="5505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -460,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:J37"/>
+  <dimension ref="A2:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -472,7 +472,7 @@
     <col min="10" max="10" width="10.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
         <v>13</v>
       </c>
@@ -498,7 +498,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -512,7 +512,7 @@
         <v>21583.9</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>15</v>
       </c>
@@ -523,7 +523,7 @@
         <v>28431.9</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B5">
         <v>20</v>
       </c>
@@ -534,7 +534,7 @@
         <v>34128.199999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>25</v>
       </c>
@@ -545,7 +545,7 @@
         <v>40851.9</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B7">
         <v>50</v>
       </c>
@@ -556,7 +556,7 @@
         <v>68779.600000000006</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B8">
         <v>75</v>
       </c>
@@ -567,7 +567,7 @@
         <v>94326.7</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B9">
         <v>100</v>
       </c>
@@ -578,7 +578,7 @@
         <v>120949</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -592,7 +592,7 @@
         <v>235610</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B11">
         <v>15</v>
       </c>
@@ -603,7 +603,7 @@
         <v>261712</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B12">
         <v>20</v>
       </c>
@@ -614,7 +614,7 @@
         <v>355920</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B13">
         <v>25</v>
       </c>
@@ -625,7 +625,7 @@
         <v>332818</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B14">
         <v>50</v>
       </c>
@@ -636,7 +636,7 @@
         <v>530397</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B15">
         <v>75</v>
       </c>
@@ -647,7 +647,7 @@
         <v>593913</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B16">
         <v>100</v>
       </c>
@@ -656,6 +656,9 @@
       </c>
       <c r="I16">
         <v>743392</v>
+      </c>
+      <c r="K16">
+        <v>698107</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
@@ -964,6 +967,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1268,6 +1272,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="AC1:AI1"/>
+    <mergeCell ref="AC2:AI2"/>
+    <mergeCell ref="AJ1:AP1"/>
+    <mergeCell ref="AJ2:AP2"/>
+    <mergeCell ref="AQ1:AW1"/>
+    <mergeCell ref="AQ2:AW2"/>
     <mergeCell ref="V1:AB1"/>
     <mergeCell ref="V2:AB2"/>
     <mergeCell ref="A1:G2"/>
@@ -1275,12 +1285,6 @@
     <mergeCell ref="H2:N2"/>
     <mergeCell ref="O1:U1"/>
     <mergeCell ref="O2:U2"/>
-    <mergeCell ref="AC1:AI1"/>
-    <mergeCell ref="AC2:AI2"/>
-    <mergeCell ref="AJ1:AP1"/>
-    <mergeCell ref="AJ2:AP2"/>
-    <mergeCell ref="AQ1:AW1"/>
-    <mergeCell ref="AQ2:AW2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1588,6 +1592,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:G2"/>
+    <mergeCell ref="H1:N1"/>
+    <mergeCell ref="O1:U1"/>
+    <mergeCell ref="V1:AB1"/>
+    <mergeCell ref="AC1:AI1"/>
     <mergeCell ref="AQ1:AW1"/>
     <mergeCell ref="H2:N2"/>
     <mergeCell ref="O2:U2"/>
@@ -1596,11 +1605,6 @@
     <mergeCell ref="AJ2:AP2"/>
     <mergeCell ref="AQ2:AW2"/>
     <mergeCell ref="AJ1:AP1"/>
-    <mergeCell ref="A1:G2"/>
-    <mergeCell ref="H1:N1"/>
-    <mergeCell ref="O1:U1"/>
-    <mergeCell ref="V1:AB1"/>
-    <mergeCell ref="AC1:AI1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
After parallelizing inner loop over community: BerkStan
</commit_message>
<xml_diff>
--- a/NewExpts/Time/Results.xlsx
+++ b/NewExpts/Time/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reetb\Desktop\Louvain-InfMax\NewExpts\Time\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C038E1-42B8-48DC-9E95-158EA68EF011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{781AFE3E-7077-4751-AE2E-7AC0BE762785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -463,13 +463,13 @@
   <dimension ref="A2:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="4" max="4" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
@@ -494,7 +494,7 @@
       <c r="I2" t="s">
         <v>19</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>20</v>
       </c>
     </row>
@@ -591,6 +591,9 @@
       <c r="I10">
         <v>235610</v>
       </c>
+      <c r="J10">
+        <v>172172</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B11">
@@ -602,6 +605,9 @@
       <c r="I11">
         <v>261712</v>
       </c>
+      <c r="J11">
+        <v>229694</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B12">
@@ -613,6 +619,9 @@
       <c r="I12">
         <v>355920</v>
       </c>
+      <c r="J12">
+        <v>263800</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B13">
@@ -624,6 +633,9 @@
       <c r="I13">
         <v>332818</v>
       </c>
+      <c r="J13">
+        <v>291804</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B14">
@@ -635,6 +647,9 @@
       <c r="I14">
         <v>530397</v>
       </c>
+      <c r="J14">
+        <v>465332</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B15">
@@ -646,6 +661,9 @@
       <c r="I15">
         <v>593913</v>
       </c>
+      <c r="J15">
+        <v>563120</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B16">
@@ -657,11 +675,11 @@
       <c r="I16">
         <v>743392</v>
       </c>
-      <c r="K16">
-        <v>698107</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J16">
+        <v>670075</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -674,11 +692,14 @@
       <c r="I17">
         <v>61912.6</v>
       </c>
-      <c r="J17" s="4">
+      <c r="J17">
+        <v>59995.7</v>
+      </c>
+      <c r="K17" s="4">
         <v>7834330</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B18">
         <v>15</v>
       </c>
@@ -688,11 +709,14 @@
       <c r="I18">
         <v>79988</v>
       </c>
-      <c r="J18" s="4">
+      <c r="J18">
+        <v>77767.399999999994</v>
+      </c>
+      <c r="K18" s="4">
         <v>7024320</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B19">
         <v>20</v>
       </c>
@@ -702,11 +726,14 @@
       <c r="I19">
         <v>96867.7</v>
       </c>
-      <c r="J19" s="4">
+      <c r="J19">
+        <v>93915.3</v>
+      </c>
+      <c r="K19" s="4">
         <v>8744330</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B20">
         <v>25</v>
       </c>
@@ -716,11 +743,14 @@
       <c r="I20">
         <v>112324</v>
       </c>
-      <c r="J20" s="4">
+      <c r="J20">
+        <v>108948</v>
+      </c>
+      <c r="K20" s="4">
         <v>7208390</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B21">
         <v>50</v>
       </c>
@@ -730,11 +760,14 @@
       <c r="I21">
         <v>186357</v>
       </c>
-      <c r="J21" s="4">
+      <c r="J21">
+        <v>180871</v>
+      </c>
+      <c r="K21" s="4">
         <v>8869170</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B22">
         <v>75</v>
       </c>
@@ -744,11 +777,14 @@
       <c r="I22">
         <v>256151</v>
       </c>
-      <c r="J22" s="4">
+      <c r="J22">
+        <v>247939</v>
+      </c>
+      <c r="K22" s="4">
         <v>8243740</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B23">
         <v>100</v>
       </c>
@@ -758,11 +794,14 @@
       <c r="I23">
         <v>319798</v>
       </c>
-      <c r="J23" s="4">
+      <c r="J23">
+        <v>311953</v>
+      </c>
+      <c r="K23" s="4">
         <v>9657590</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -776,10 +815,13 @@
         <v>24336.799999999999</v>
       </c>
       <c r="J24">
+        <v>23543</v>
+      </c>
+      <c r="K24">
         <v>876604</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B25">
         <v>15</v>
       </c>
@@ -790,10 +832,13 @@
         <v>31039.1</v>
       </c>
       <c r="J25">
+        <v>29408.2</v>
+      </c>
+      <c r="K25">
         <v>863160</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B26">
         <v>20</v>
       </c>
@@ -804,10 +849,13 @@
         <v>38126.6</v>
       </c>
       <c r="J26">
+        <v>35878.9</v>
+      </c>
+      <c r="K26">
         <v>861731</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B27">
         <v>25</v>
       </c>
@@ -818,10 +866,13 @@
         <v>45069.7</v>
       </c>
       <c r="J27">
+        <v>41530.800000000003</v>
+      </c>
+      <c r="K27">
         <v>870060</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B28">
         <v>50</v>
       </c>
@@ -832,10 +883,13 @@
         <v>75724.600000000006</v>
       </c>
       <c r="J28">
+        <v>71455</v>
+      </c>
+      <c r="K28">
         <v>974436</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B29">
         <v>75</v>
       </c>
@@ -845,11 +899,14 @@
       <c r="I29">
         <v>105496</v>
       </c>
-      <c r="J29" s="4">
+      <c r="J29">
+        <v>99399.8</v>
+      </c>
+      <c r="K29" s="4">
         <v>1156990</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B30">
         <v>100</v>
       </c>
@@ -859,11 +916,14 @@
       <c r="I30">
         <v>129107</v>
       </c>
-      <c r="J30" s="4">
+      <c r="J30">
+        <v>126985</v>
+      </c>
+      <c r="K30" s="4">
         <v>1317000</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -877,10 +937,13 @@
         <v>55810.3</v>
       </c>
       <c r="J31">
+        <v>56130.3</v>
+      </c>
+      <c r="K31">
         <v>610519</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B32">
         <v>15</v>
       </c>
@@ -891,10 +954,13 @@
         <v>84581.6</v>
       </c>
       <c r="J32">
+        <v>78948.800000000003</v>
+      </c>
+      <c r="K32">
         <v>750901</v>
       </c>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B33">
         <v>20</v>
       </c>
@@ -905,10 +971,13 @@
         <v>101797</v>
       </c>
       <c r="J33">
+        <v>99577</v>
+      </c>
+      <c r="K33">
         <v>877541</v>
       </c>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B34">
         <v>25</v>
       </c>
@@ -918,11 +987,14 @@
       <c r="I34">
         <v>126085</v>
       </c>
-      <c r="J34" s="4">
+      <c r="J34">
+        <v>119859</v>
+      </c>
+      <c r="K34" s="4">
         <v>1006810</v>
       </c>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B35">
         <v>50</v>
       </c>
@@ -932,11 +1004,14 @@
       <c r="I35">
         <v>204407</v>
       </c>
-      <c r="J35" s="4">
+      <c r="J35">
+        <v>211838</v>
+      </c>
+      <c r="K35" s="4">
         <v>1773040</v>
       </c>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B36">
         <v>75</v>
       </c>
@@ -946,11 +1021,14 @@
       <c r="I36">
         <v>292055</v>
       </c>
-      <c r="J36" s="4">
+      <c r="J36">
+        <v>304155</v>
+      </c>
+      <c r="K36" s="4">
         <v>2296560</v>
       </c>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B37">
         <v>100</v>
       </c>
@@ -960,7 +1038,10 @@
       <c r="I37">
         <v>395949</v>
       </c>
-      <c r="J37" s="4">
+      <c r="J37">
+        <v>380922</v>
+      </c>
+      <c r="K37" s="4">
         <v>3100730</v>
       </c>
     </row>
@@ -1272,12 +1353,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="AC1:AI1"/>
-    <mergeCell ref="AC2:AI2"/>
-    <mergeCell ref="AJ1:AP1"/>
-    <mergeCell ref="AJ2:AP2"/>
-    <mergeCell ref="AQ1:AW1"/>
-    <mergeCell ref="AQ2:AW2"/>
     <mergeCell ref="V1:AB1"/>
     <mergeCell ref="V2:AB2"/>
     <mergeCell ref="A1:G2"/>
@@ -1285,6 +1360,12 @@
     <mergeCell ref="H2:N2"/>
     <mergeCell ref="O1:U1"/>
     <mergeCell ref="O2:U2"/>
+    <mergeCell ref="AC1:AI1"/>
+    <mergeCell ref="AC2:AI2"/>
+    <mergeCell ref="AJ1:AP1"/>
+    <mergeCell ref="AJ2:AP2"/>
+    <mergeCell ref="AQ1:AW1"/>
+    <mergeCell ref="AQ2:AW2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1592,11 +1673,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:G2"/>
-    <mergeCell ref="H1:N1"/>
-    <mergeCell ref="O1:U1"/>
-    <mergeCell ref="V1:AB1"/>
-    <mergeCell ref="AC1:AI1"/>
     <mergeCell ref="AQ1:AW1"/>
     <mergeCell ref="H2:N2"/>
     <mergeCell ref="O2:U2"/>
@@ -1605,6 +1681,11 @@
     <mergeCell ref="AJ2:AP2"/>
     <mergeCell ref="AQ2:AW2"/>
     <mergeCell ref="AJ1:AP1"/>
+    <mergeCell ref="A1:G2"/>
+    <mergeCell ref="H1:N1"/>
+    <mergeCell ref="O1:U1"/>
+    <mergeCell ref="V1:AB1"/>
+    <mergeCell ref="AC1:AI1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adjusted Sampling expected spread and time for BerkStan
</commit_message>
<xml_diff>
--- a/NewExpts/Time/Results.xlsx
+++ b/NewExpts/Time/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reetb\Desktop\Louvain-InfMax\NewExpts\Time\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{781AFE3E-7077-4751-AE2E-7AC0BE762785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A08CD2-9594-40A7-96FB-5F9B5E8160A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9600" yWindow="1680" windowWidth="57600" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -460,19 +460,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:K37"/>
+  <dimension ref="A2:M37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+      <selection activeCell="K31" sqref="K31:K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="4" max="4" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
         <v>13</v>
       </c>
@@ -494,11 +494,11 @@
       <c r="I2" t="s">
         <v>19</v>
       </c>
-      <c r="K2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -512,7 +512,7 @@
         <v>21583.9</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>15</v>
       </c>
@@ -523,7 +523,7 @@
         <v>28431.9</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B5">
         <v>20</v>
       </c>
@@ -534,7 +534,7 @@
         <v>34128.199999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>25</v>
       </c>
@@ -545,7 +545,7 @@
         <v>40851.9</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B7">
         <v>50</v>
       </c>
@@ -556,7 +556,7 @@
         <v>68779.600000000006</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B8">
         <v>75</v>
       </c>
@@ -567,7 +567,7 @@
         <v>94326.7</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B9">
         <v>100</v>
       </c>
@@ -578,7 +578,7 @@
         <v>120949</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -595,7 +595,7 @@
         <v>172172</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B11">
         <v>15</v>
       </c>
@@ -609,7 +609,7 @@
         <v>229694</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B12">
         <v>20</v>
       </c>
@@ -623,7 +623,7 @@
         <v>263800</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B13">
         <v>25</v>
       </c>
@@ -637,7 +637,7 @@
         <v>291804</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B14">
         <v>50</v>
       </c>
@@ -651,7 +651,7 @@
         <v>465332</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B15">
         <v>75</v>
       </c>
@@ -665,7 +665,7 @@
         <v>563120</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B16">
         <v>100</v>
       </c>
@@ -679,7 +679,7 @@
         <v>670075</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -695,11 +695,14 @@
       <c r="J17">
         <v>59995.7</v>
       </c>
-      <c r="K17" s="4">
+      <c r="K17">
+        <v>27677</v>
+      </c>
+      <c r="L17" s="4">
         <v>7834330</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B18">
         <v>15</v>
       </c>
@@ -712,11 +715,14 @@
       <c r="J18">
         <v>77767.399999999994</v>
       </c>
-      <c r="K18" s="4">
+      <c r="K18">
+        <v>32239.7</v>
+      </c>
+      <c r="L18" s="4">
         <v>7024320</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B19">
         <v>20</v>
       </c>
@@ -729,11 +735,14 @@
       <c r="J19">
         <v>93915.3</v>
       </c>
-      <c r="K19" s="4">
+      <c r="K19">
+        <v>41193.1</v>
+      </c>
+      <c r="L19" s="4">
         <v>8744330</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B20">
         <v>25</v>
       </c>
@@ -746,11 +755,14 @@
       <c r="J20">
         <v>108948</v>
       </c>
-      <c r="K20" s="4">
+      <c r="K20">
+        <v>45251.9</v>
+      </c>
+      <c r="L20" s="4">
         <v>7208390</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B21">
         <v>50</v>
       </c>
@@ -763,11 +775,14 @@
       <c r="J21">
         <v>180871</v>
       </c>
-      <c r="K21" s="4">
+      <c r="K21">
+        <v>67066.899999999994</v>
+      </c>
+      <c r="L21" s="4">
         <v>8869170</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B22">
         <v>75</v>
       </c>
@@ -780,11 +795,14 @@
       <c r="J22">
         <v>247939</v>
       </c>
-      <c r="K22" s="4">
+      <c r="K22">
+        <v>86603.3</v>
+      </c>
+      <c r="L22" s="4">
         <v>8243740</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B23">
         <v>100</v>
       </c>
@@ -797,11 +815,14 @@
       <c r="J23">
         <v>311953</v>
       </c>
-      <c r="K23" s="4">
+      <c r="K23">
+        <v>109224</v>
+      </c>
+      <c r="L23" s="4">
         <v>9657590</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -818,10 +839,13 @@
         <v>23543</v>
       </c>
       <c r="K24">
+        <v>7941.29</v>
+      </c>
+      <c r="L24">
         <v>876604</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B25">
         <v>15</v>
       </c>
@@ -835,10 +859,13 @@
         <v>29408.2</v>
       </c>
       <c r="K25">
+        <v>7966.33</v>
+      </c>
+      <c r="L25">
         <v>863160</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B26">
         <v>20</v>
       </c>
@@ -852,10 +879,13 @@
         <v>35878.9</v>
       </c>
       <c r="K26">
+        <v>10201.9</v>
+      </c>
+      <c r="L26">
         <v>861731</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B27">
         <v>25</v>
       </c>
@@ -869,10 +899,13 @@
         <v>41530.800000000003</v>
       </c>
       <c r="K27">
+        <v>10075.299999999999</v>
+      </c>
+      <c r="L27">
         <v>870060</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B28">
         <v>50</v>
       </c>
@@ -886,10 +919,13 @@
         <v>71455</v>
       </c>
       <c r="K28">
+        <v>13542.3</v>
+      </c>
+      <c r="L28">
         <v>974436</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B29">
         <v>75</v>
       </c>
@@ -902,11 +938,14 @@
       <c r="J29">
         <v>99399.8</v>
       </c>
-      <c r="K29" s="4">
+      <c r="K29">
+        <v>15679.6</v>
+      </c>
+      <c r="L29" s="4">
         <v>1156990</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B30">
         <v>100</v>
       </c>
@@ -919,11 +958,14 @@
       <c r="J30">
         <v>126985</v>
       </c>
-      <c r="K30" s="4">
+      <c r="K30">
+        <v>18982.099999999999</v>
+      </c>
+      <c r="L30" s="4">
         <v>1317000</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -940,10 +982,13 @@
         <v>56130.3</v>
       </c>
       <c r="K31">
+        <v>7616.64</v>
+      </c>
+      <c r="L31">
         <v>610519</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B32">
         <v>15</v>
       </c>
@@ -957,10 +1002,13 @@
         <v>78948.800000000003</v>
       </c>
       <c r="K32">
+        <v>7574.11</v>
+      </c>
+      <c r="L32">
         <v>750901</v>
       </c>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B33">
         <v>20</v>
       </c>
@@ -974,10 +1022,13 @@
         <v>99577</v>
       </c>
       <c r="K33">
+        <v>7925.11</v>
+      </c>
+      <c r="L33">
         <v>877541</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B34">
         <v>25</v>
       </c>
@@ -990,11 +1041,14 @@
       <c r="J34">
         <v>119859</v>
       </c>
-      <c r="K34" s="4">
+      <c r="K34">
+        <v>7496.6</v>
+      </c>
+      <c r="L34" s="4">
         <v>1006810</v>
       </c>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B35">
         <v>50</v>
       </c>
@@ -1007,11 +1061,14 @@
       <c r="J35">
         <v>211838</v>
       </c>
-      <c r="K35" s="4">
+      <c r="K35">
+        <v>7731.6</v>
+      </c>
+      <c r="L35" s="4">
         <v>1773040</v>
       </c>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B36">
         <v>75</v>
       </c>
@@ -1024,11 +1081,14 @@
       <c r="J36">
         <v>304155</v>
       </c>
-      <c r="K36" s="4">
+      <c r="K36">
+        <v>7571.6</v>
+      </c>
+      <c r="L36" s="4">
         <v>2296560</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B37">
         <v>100</v>
       </c>
@@ -1041,8 +1101,14 @@
       <c r="J37">
         <v>380922</v>
       </c>
-      <c r="K37" s="4">
+      <c r="K37">
+        <v>7950.87</v>
+      </c>
+      <c r="L37" s="4">
         <v>3100730</v>
+      </c>
+      <c r="M37" s="4">
+        <v>1121140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>